<commit_message>
_learning over time & fix choose_wrong & fix distcomp_
</commit_message>
<xml_diff>
--- a/Tables/repeat_loans.xlsx
+++ b/Tables/repeat_loans.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isaac\Dropbox\Apps\ShareLaTeX\Donde2020\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE964C84-66E6-4D7A-8865-4F198083657F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E235F35-A7BB-4E59-AED2-5A9695E27FE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-8190" windowWidth="29040" windowHeight="15720" xr2:uid="{4D4440F4-6748-4F85-9413-7DB268D90AD8}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{4D4440F4-6748-4F85-9413-7DB268D90AD8}"/>
   </bookViews>
   <sheets>
     <sheet name="repeat_loans" sheetId="1" r:id="rId1"/>
@@ -55,22 +55,22 @@
     <t xml:space="preserve">Days from 1st loan </t>
   </si>
   <si>
-    <t>Cond. on repaying</t>
-  </si>
-  <si>
     <t>Cond. on default</t>
   </si>
   <si>
     <t>Different collateral</t>
   </si>
   <si>
-    <t>After recovery</t>
+    <t>Ever pawns again (ITT)</t>
   </si>
   <si>
-    <t>Before recovery</t>
+    <t>Cond. on rec</t>
   </si>
   <si>
-    <t>Ever pawns again (ITT)</t>
+    <t>After 90 days</t>
+  </si>
+  <si>
+    <t>Within 90 days</t>
   </si>
 </sst>
 </file>
@@ -149,9 +149,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -166,6 +163,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -233,10 +233,10 @@
             <v>0.034</v>
           </cell>
           <cell r="F5" t="str">
-            <v>0.050***</v>
+            <v>0.029***</v>
           </cell>
           <cell r="G5" t="str">
-            <v>0.0090</v>
+            <v>0.032</v>
           </cell>
           <cell r="H5" t="str">
             <v>6.76***</v>
@@ -259,10 +259,10 @@
             <v>(0.027)</v>
           </cell>
           <cell r="F6" t="str">
-            <v>(0.014)</v>
+            <v>(0.0086)</v>
           </cell>
           <cell r="G6" t="str">
-            <v>(0.026)</v>
+            <v>(0.028)</v>
           </cell>
           <cell r="H6" t="str">
             <v>(2.42)</v>
@@ -282,10 +282,10 @@
             <v>0.024</v>
           </cell>
           <cell r="F8" t="str">
-            <v>0.013</v>
+            <v>0.0047</v>
           </cell>
           <cell r="G8" t="str">
-            <v>0.022</v>
+            <v>0.030</v>
           </cell>
           <cell r="H8" t="str">
             <v>0.92</v>
@@ -308,10 +308,10 @@
             <v>(0.025)</v>
           </cell>
           <cell r="F9" t="str">
-            <v>(0.0095)</v>
+            <v>(0.0048)</v>
           </cell>
           <cell r="G9" t="str">
-            <v>(0.025)</v>
+            <v>(0.027)</v>
           </cell>
           <cell r="H9" t="str">
             <v>(1.94)</v>
@@ -357,7 +357,7 @@
             <v>0.008</v>
           </cell>
           <cell r="G12" t="str">
-            <v>0.000</v>
+            <v>0.001</v>
           </cell>
           <cell r="H12" t="str">
             <v>0.012</v>
@@ -380,10 +380,10 @@
             <v>0.27</v>
           </cell>
           <cell r="F13" t="str">
-            <v>0.032</v>
+            <v>0.0081</v>
           </cell>
           <cell r="G13" t="str">
-            <v>0.27</v>
+            <v>0.30</v>
           </cell>
           <cell r="H13" t="str">
             <v>30.1</v>
@@ -712,80 +712,80 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="3"/>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
+      <c r="A1" s="2"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
     </row>
     <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
+      <c r="B2" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
     </row>
     <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="4"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8" t="s">
+      <c r="A3" s="3"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="E3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" s="8" t="s">
+      <c r="F3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8" t="s">
+      <c r="G3" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="5" t="str">
+      <c r="A4" s="4" t="str">
         <f>[1]repeat_loans!A2</f>
         <v/>
       </c>
-      <c r="B4" s="9" t="str">
+      <c r="B4" s="8" t="str">
         <f>[1]repeat_loans!B2</f>
         <v>(1)</v>
       </c>
-      <c r="C4" s="9" t="str">
+      <c r="C4" s="8" t="str">
         <f>[1]repeat_loans!C2</f>
         <v>(2)</v>
       </c>
-      <c r="D4" s="9" t="str">
+      <c r="D4" s="8" t="str">
         <f>[1]repeat_loans!D2</f>
         <v>(3)</v>
       </c>
-      <c r="E4" s="9" t="str">
+      <c r="E4" s="8" t="str">
         <f>[1]repeat_loans!E2</f>
         <v>(4)</v>
       </c>
-      <c r="F4" s="9" t="str">
+      <c r="F4" s="8" t="str">
         <f>[1]repeat_loans!F2</f>
         <v>(5)</v>
       </c>
-      <c r="G4" s="9" t="str">
+      <c r="G4" s="8" t="str">
         <f>[1]repeat_loans!G2</f>
         <v>(6)</v>
       </c>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9" t="str">
+      <c r="H4" s="8"/>
+      <c r="I4" s="8" t="str">
         <f>[1]repeat_loans!H2</f>
         <v>(7)</v>
       </c>
@@ -812,11 +812,11 @@
       </c>
       <c r="F5" s="1" t="str">
         <f>[1]repeat_loans!F5</f>
-        <v>0.050***</v>
+        <v>0.029***</v>
       </c>
       <c r="G5" s="1" t="str">
         <f>[1]repeat_loans!G5</f>
-        <v>0.0090</v>
+        <v>0.032</v>
       </c>
       <c r="I5" s="1" t="str">
         <f>[1]repeat_loans!H5</f>
@@ -846,11 +846,11 @@
       </c>
       <c r="F6" s="1" t="str">
         <f>[1]repeat_loans!F6</f>
-        <v>(0.014)</v>
+        <v>(0.0086)</v>
       </c>
       <c r="G6" s="1" t="str">
         <f>[1]repeat_loans!G6</f>
-        <v>(0.026)</v>
+        <v>(0.028)</v>
       </c>
       <c r="I6" s="1" t="str">
         <f>[1]repeat_loans!H6</f>
@@ -879,11 +879,11 @@
       </c>
       <c r="F7" s="1" t="str">
         <f>[1]repeat_loans!F8</f>
-        <v>0.013</v>
+        <v>0.0047</v>
       </c>
       <c r="G7" s="1" t="str">
         <f>[1]repeat_loans!G8</f>
-        <v>0.022</v>
+        <v>0.030</v>
       </c>
       <c r="I7" s="1" t="str">
         <f>[1]repeat_loans!H8</f>
@@ -913,11 +913,11 @@
       </c>
       <c r="F8" s="1" t="str">
         <f>[1]repeat_loans!F9</f>
-        <v>(0.0095)</v>
+        <v>(0.0048)</v>
       </c>
       <c r="G8" s="1" t="str">
         <f>[1]repeat_loans!G9</f>
-        <v>(0.025)</v>
+        <v>(0.027)</v>
       </c>
       <c r="I8" s="1" t="str">
         <f>[1]repeat_loans!H9</f>
@@ -925,35 +925,35 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="10" t="str">
+      <c r="B10" s="9" t="str">
         <f>[1]repeat_loans!B11</f>
         <v>4441</v>
       </c>
-      <c r="C10" s="10" t="str">
+      <c r="C10" s="9" t="str">
         <f>[1]repeat_loans!C11</f>
         <v>2102</v>
       </c>
-      <c r="D10" s="10" t="str">
+      <c r="D10" s="9" t="str">
         <f>[1]repeat_loans!D11</f>
         <v>2339</v>
       </c>
-      <c r="E10" s="10" t="str">
+      <c r="E10" s="9" t="str">
         <f>[1]repeat_loans!E11</f>
         <v>4441</v>
       </c>
-      <c r="F10" s="10" t="str">
+      <c r="F10" s="9" t="str">
         <f>[1]repeat_loans!F11</f>
         <v>4441</v>
       </c>
-      <c r="G10" s="10" t="str">
+      <c r="G10" s="9" t="str">
         <f>[1]repeat_loans!G11</f>
         <v>4441</v>
       </c>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10" t="str">
+      <c r="H10" s="9"/>
+      <c r="I10" s="9" t="str">
         <f>[1]repeat_loans!H11</f>
         <v>1493</v>
       </c>
@@ -984,7 +984,7 @@
       </c>
       <c r="G11" s="1" t="str">
         <f>[1]repeat_loans!G12</f>
-        <v>0.000</v>
+        <v>0.001</v>
       </c>
       <c r="I11" s="1" t="str">
         <f>[1]repeat_loans!H12</f>
@@ -992,36 +992,36 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="4" t="str">
+      <c r="A12" s="3" t="str">
         <f>[1]repeat_loans!A13</f>
         <v>Control Mean</v>
       </c>
-      <c r="B12" s="8" t="str">
+      <c r="B12" s="7" t="str">
         <f>[1]repeat_loans!B13</f>
         <v>0.30</v>
       </c>
-      <c r="C12" s="8" t="str">
+      <c r="C12" s="7" t="str">
         <f>[1]repeat_loans!C13</f>
         <v>0.33</v>
       </c>
-      <c r="D12" s="8" t="str">
+      <c r="D12" s="7" t="str">
         <f>[1]repeat_loans!D13</f>
         <v>0.28</v>
       </c>
-      <c r="E12" s="8" t="str">
+      <c r="E12" s="7" t="str">
         <f>[1]repeat_loans!E13</f>
         <v>0.27</v>
       </c>
-      <c r="F12" s="8" t="str">
+      <c r="F12" s="7" t="str">
         <f>[1]repeat_loans!F13</f>
-        <v>0.032</v>
-      </c>
-      <c r="G12" s="8" t="str">
+        <v>0.0081</v>
+      </c>
+      <c r="G12" s="7" t="str">
         <f>[1]repeat_loans!G13</f>
-        <v>0.27</v>
-      </c>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8" t="str">
+        <v>0.30</v>
+      </c>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7" t="str">
         <f>[1]repeat_loans!H13</f>
         <v>30.1</v>
       </c>

</xml_diff>

<commit_message>
computation of lenders profit + minor edits
</commit_message>
<xml_diff>
--- a/Tables/repeat_loans.xlsx
+++ b/Tables/repeat_loans.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isaac\Dropbox\Apps\Overleaf\Donde2022\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CB2F66E-18D8-4C93-B5DC-5E9E5AA7B811}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46F301BD-503B-4B29-98BC-9EDE4BCE1B75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19515" yWindow="-13395" windowWidth="19245" windowHeight="9285" xr2:uid="{4D4440F4-6748-4F85-9413-7DB268D90AD8}"/>
+    <workbookView xWindow="-28920" yWindow="-9735" windowWidth="29040" windowHeight="15720" xr2:uid="{4D4440F4-6748-4F85-9413-7DB268D90AD8}"/>
   </bookViews>
   <sheets>
     <sheet name="repeat_loans" sheetId="1" r:id="rId1"/>
@@ -88,7 +88,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -136,11 +136,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -160,7 +169,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -213,16 +226,16 @@
         </row>
         <row r="5">
           <cell r="B5" t="str">
-            <v>0.063</v>
+            <v>0.067*</v>
           </cell>
           <cell r="C5" t="str">
-            <v>0.041***</v>
+            <v>0.037***</v>
           </cell>
           <cell r="D5" t="str">
-            <v>0.024</v>
+            <v>0.032</v>
           </cell>
           <cell r="E5" t="str">
-            <v>0.042</v>
+            <v>0.044</v>
           </cell>
           <cell r="F5" t="str">
             <v>0.11**</v>
@@ -233,36 +246,36 @@
             <v/>
           </cell>
           <cell r="B6" t="str">
-            <v>(0.043)</v>
+            <v>(0.035)</v>
           </cell>
           <cell r="C6" t="str">
             <v>(0.013)</v>
           </cell>
           <cell r="D6" t="str">
-            <v>(0.033)</v>
+            <v>(0.027)</v>
           </cell>
           <cell r="E6" t="str">
-            <v>(0.038)</v>
+            <v>(0.030)</v>
           </cell>
           <cell r="F6" t="str">
-            <v>(0.055)</v>
+            <v>(0.047)</v>
           </cell>
         </row>
         <row r="8">
           <cell r="B8" t="str">
-            <v>0.050</v>
+            <v>0.040</v>
           </cell>
           <cell r="C8" t="str">
-            <v>0.022*</v>
+            <v>0.0098</v>
           </cell>
           <cell r="D8" t="str">
-            <v>0.028</v>
+            <v>0.030</v>
           </cell>
           <cell r="E8" t="str">
-            <v>0.043</v>
+            <v>0.038</v>
           </cell>
           <cell r="F8" t="str">
-            <v>0.088*</v>
+            <v>0.057</v>
           </cell>
         </row>
         <row r="9">
@@ -270,36 +283,36 @@
             <v/>
           </cell>
           <cell r="B9" t="str">
-            <v>(0.036)</v>
+            <v>(0.031)</v>
           </cell>
           <cell r="C9" t="str">
-            <v>(0.011)</v>
+            <v>(0.0087)</v>
           </cell>
           <cell r="D9" t="str">
-            <v>(0.031)</v>
+            <v>(0.026)</v>
           </cell>
           <cell r="E9" t="str">
-            <v>(0.033)</v>
+            <v>(0.028)</v>
           </cell>
           <cell r="F9" t="str">
-            <v>(0.045)</v>
+            <v>(0.042)</v>
           </cell>
         </row>
         <row r="11">
           <cell r="B11" t="str">
-            <v>6302</v>
+            <v>4441</v>
           </cell>
           <cell r="C11" t="str">
-            <v>6302</v>
+            <v>4441</v>
           </cell>
           <cell r="D11" t="str">
-            <v>6302</v>
+            <v>4441</v>
           </cell>
           <cell r="E11" t="str">
-            <v>6302</v>
+            <v>4441</v>
           </cell>
           <cell r="F11" t="str">
-            <v>3032</v>
+            <v>2170</v>
           </cell>
         </row>
         <row r="12">
@@ -307,7 +320,7 @@
             <v>0.003</v>
           </cell>
           <cell r="C12" t="str">
-            <v>0.007</v>
+            <v>0.006</v>
           </cell>
           <cell r="D12" t="str">
             <v>0.001</v>
@@ -324,19 +337,19 @@
             <v>Control Mean</v>
           </cell>
           <cell r="B13" t="str">
-            <v>0.34</v>
+            <v>0.32</v>
           </cell>
           <cell r="C13" t="str">
-            <v>0.018</v>
+            <v>0.020</v>
           </cell>
           <cell r="D13" t="str">
-            <v>0.32</v>
+            <v>0.30</v>
           </cell>
           <cell r="E13" t="str">
-            <v>0.32</v>
+            <v>0.30</v>
           </cell>
           <cell r="F13" t="str">
-            <v>0.36</v>
+            <v>0.35</v>
           </cell>
         </row>
       </sheetData>
@@ -346,9 +359,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -386,7 +399,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -492,7 +505,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -634,7 +647,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -642,7 +655,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B8CDD8A-A5B9-4973-A3CC-B413497D22BE}">
-  <dimension ref="A2:F13"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:F12"/>
@@ -654,27 +667,36 @@
     <col min="2" max="2" width="9.54296875" style="1" customWidth="1"/>
     <col min="3" max="3" width="16.453125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.1796875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10" customWidth="1"/>
+    <col min="7" max="7" width="11.7265625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="10"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="10"/>
+    </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="4"/>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
     </row>
     <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="2"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8" t="s">
+      <c r="B3" s="5"/>
+      <c r="C3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="8" t="s">
@@ -716,19 +738,19 @@
       </c>
       <c r="B5" s="1" t="str">
         <f>[1]repeat_loans!B5</f>
-        <v>0.063</v>
+        <v>0.067*</v>
       </c>
       <c r="C5" s="1" t="str">
         <f>[1]repeat_loans!C5</f>
-        <v>0.041***</v>
+        <v>0.037***</v>
       </c>
       <c r="D5" s="1" t="str">
         <f>[1]repeat_loans!D5</f>
-        <v>0.024</v>
+        <v>0.032</v>
       </c>
       <c r="E5" s="1" t="str">
         <f>[1]repeat_loans!E5</f>
-        <v>0.042</v>
+        <v>0.044</v>
       </c>
       <c r="F5" s="1" t="str">
         <f>[1]repeat_loans!F5</f>
@@ -742,7 +764,7 @@
       </c>
       <c r="B6" s="1" t="str">
         <f>[1]repeat_loans!B6</f>
-        <v>(0.043)</v>
+        <v>(0.035)</v>
       </c>
       <c r="C6" s="1" t="str">
         <f>[1]repeat_loans!C6</f>
@@ -750,15 +772,15 @@
       </c>
       <c r="D6" s="1" t="str">
         <f>[1]repeat_loans!D6</f>
-        <v>(0.033)</v>
+        <v>(0.027)</v>
       </c>
       <c r="E6" s="1" t="str">
         <f>[1]repeat_loans!E6</f>
-        <v>(0.038)</v>
+        <v>(0.030)</v>
       </c>
       <c r="F6" s="1" t="str">
         <f>[1]repeat_loans!F6</f>
-        <v>(0.055)</v>
+        <v>(0.047)</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
@@ -767,23 +789,23 @@
       </c>
       <c r="B7" s="1" t="str">
         <f>[1]repeat_loans!B8</f>
-        <v>0.050</v>
+        <v>0.040</v>
       </c>
       <c r="C7" s="1" t="str">
         <f>[1]repeat_loans!C8</f>
-        <v>0.022*</v>
+        <v>0.0098</v>
       </c>
       <c r="D7" s="1" t="str">
         <f>[1]repeat_loans!D8</f>
-        <v>0.028</v>
+        <v>0.030</v>
       </c>
       <c r="E7" s="1" t="str">
         <f>[1]repeat_loans!E8</f>
-        <v>0.043</v>
+        <v>0.038</v>
       </c>
       <c r="F7" s="1" t="str">
         <f>[1]repeat_loans!F8</f>
-        <v>0.088*</v>
+        <v>0.057</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
@@ -793,24 +815,27 @@
       </c>
       <c r="B8" s="1" t="str">
         <f>[1]repeat_loans!B9</f>
-        <v>(0.036)</v>
+        <v>(0.031)</v>
       </c>
       <c r="C8" s="1" t="str">
         <f>[1]repeat_loans!C9</f>
-        <v>(0.011)</v>
+        <v>(0.0087)</v>
       </c>
       <c r="D8" s="1" t="str">
         <f>[1]repeat_loans!D9</f>
-        <v>(0.031)</v>
+        <v>(0.026)</v>
       </c>
       <c r="E8" s="1" t="str">
         <f>[1]repeat_loans!E9</f>
-        <v>(0.033)</v>
+        <v>(0.028)</v>
       </c>
       <c r="F8" s="1" t="str">
         <f>[1]repeat_loans!F9</f>
-        <v>(0.045)</v>
-      </c>
+        <v>(0.042)</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
@@ -818,23 +843,23 @@
       </c>
       <c r="B10" s="7" t="str">
         <f>[1]repeat_loans!B11</f>
-        <v>6302</v>
+        <v>4441</v>
       </c>
       <c r="C10" s="7" t="str">
         <f>[1]repeat_loans!C11</f>
-        <v>6302</v>
+        <v>4441</v>
       </c>
       <c r="D10" s="7" t="str">
         <f>[1]repeat_loans!D11</f>
-        <v>6302</v>
+        <v>4441</v>
       </c>
       <c r="E10" s="7" t="str">
         <f>[1]repeat_loans!E11</f>
-        <v>6302</v>
+        <v>4441</v>
       </c>
       <c r="F10" s="7" t="str">
         <f>[1]repeat_loans!F11</f>
-        <v>3032</v>
+        <v>2170</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
@@ -847,7 +872,7 @@
       </c>
       <c r="C11" s="1" t="str">
         <f>[1]repeat_loans!C12</f>
-        <v>0.007</v>
+        <v>0.006</v>
       </c>
       <c r="D11" s="1" t="str">
         <f>[1]repeat_loans!D12</f>
@@ -869,23 +894,23 @@
       </c>
       <c r="B12" s="5" t="str">
         <f>[1]repeat_loans!B13</f>
-        <v>0.34</v>
+        <v>0.32</v>
       </c>
       <c r="C12" s="5" t="str">
         <f>[1]repeat_loans!C13</f>
-        <v>0.018</v>
+        <v>0.020</v>
       </c>
       <c r="D12" s="5" t="str">
         <f>[1]repeat_loans!D13</f>
-        <v>0.32</v>
+        <v>0.30</v>
       </c>
       <c r="E12" s="5" t="str">
         <f>[1]repeat_loans!E13</f>
-        <v>0.32</v>
+        <v>0.30</v>
       </c>
       <c r="F12" s="5" t="str">
         <f>[1]repeat_loans!F13</f>
-        <v>0.36</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>

</xml_diff>